<commit_message>
rebuilding site Thu Feb 24 07:00:25     2022
</commit_message>
<xml_diff>
--- a/样书_作者(1).xlsx
+++ b/样书_作者(1).xlsx
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="42" uniqueCount="35">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="42" uniqueCount="39">
   <si>
     <t>ISBN</t>
   </si>
@@ -63,7 +63,19 @@
     <t>赵佳霓</t>
   </si>
   <si>
-    <r>
+    <t>伏晓梅</t>
+  </si>
+  <si>
+    <t>浙江省杭州市滨江区东莞社区6号</t>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FF333333"/>
+        <rFont val="Microsoft YaHei UI"/>
+        <charset val="134"/>
+      </rPr>
       <t>Vue+Spring Boot</t>
     </r>
     <r>
@@ -130,6 +142,53 @@
     </r>
   </si>
   <si>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FF333333"/>
+        <rFont val="Microsoft YaHei UI"/>
+        <charset val="134"/>
+      </rPr>
+      <t>HoloLens 2</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FF333333"/>
+        <rFont val="宋体"/>
+        <charset val="134"/>
+      </rPr>
+      <t>开发入门精要——基于</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FF333333"/>
+        <rFont val="Microsoft YaHei UI"/>
+        <charset val="134"/>
+      </rPr>
+      <t>Unity</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FF333333"/>
+        <rFont val="宋体"/>
+        <charset val="134"/>
+      </rPr>
+      <t>和</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FF333333"/>
+        <rFont val="Microsoft YaHei UI"/>
+        <charset val="134"/>
+      </rPr>
+      <t>MRTK</t>
+    </r>
+  </si>
+  <si>
     <t>胡峰</t>
   </si>
   <si>
@@ -159,6 +218,36 @@
     </r>
   </si>
   <si>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FF333333"/>
+        <rFont val="宋体"/>
+        <charset val="134"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>华为</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FF333333"/>
+        <rFont val="Microsoft YaHei UI"/>
+        <charset val="134"/>
+      </rPr>
+      <t>HCIA</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FF333333"/>
+        <rFont val="宋体"/>
+        <charset val="134"/>
+      </rPr>
+      <t>路由与交换技术实战</t>
+    </r>
+  </si>
+  <si>
     <t>江威</t>
   </si>
   <si>
@@ -166,6 +255,12 @@
   </si>
   <si>
     <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FF333333"/>
+        <rFont val="Microsoft YaHei UI"/>
+        <charset val="134"/>
+      </rPr>
       <t>Flutter</t>
     </r>
     <r>
@@ -185,32 +280,8 @@
     <t xml:space="preserve">北京市丰台区和义东里小区一区8楼1单元302 </t>
   </si>
   <si>
-    <t>Python异步编程实战——基于AIO的全栈开发技术</t>
-  </si>
-  <si>
-    <t>陈启豪</t>
-  </si>
-  <si>
-    <t>广州市黄埔区萝岗和苑A4-2602</t>
-  </si>
-  <si>
-    <t>黄晓锐</t>
-  </si>
-  <si>
-    <t>福建省厦门市思明区金尚路23之2  205</t>
-  </si>
-  <si>
-    <r>
-      <t>全栈</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color rgb="FF333333"/>
-        <rFont val="Microsoft YaHei UI"/>
-        <charset val="134"/>
-      </rPr>
-      <t>UI</t>
+    <r>
+      <t>Flutter</t>
     </r>
     <r>
       <rPr>
@@ -219,8 +290,23 @@
         <rFont val="宋体"/>
         <charset val="134"/>
       </rPr>
-      <t>自动化测试实战</t>
-    </r>
+      <t>实战指南</t>
+    </r>
+  </si>
+  <si>
+    <t>Python异步编程实战——基于AIO的全栈开发技术</t>
+  </si>
+  <si>
+    <t>陈启豪</t>
+  </si>
+  <si>
+    <t>广州市黄埔区萝岗和苑A4-2602</t>
+  </si>
+  <si>
+    <t>黄晓锐</t>
+  </si>
+  <si>
+    <t>福建省厦门市思明区金尚路23之2  205</t>
   </si>
 </sst>
 </file>
@@ -228,13 +314,13 @@
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <numFmts count="5">
+    <numFmt numFmtId="41" formatCode="_ * #,##0_ ;_ * \-#,##0_ ;_ * &quot;-&quot;_ ;_ @_ "/>
+    <numFmt numFmtId="44" formatCode="_ &quot;￥&quot;* #,##0.00_ ;_ &quot;￥&quot;* \-#,##0.00_ ;_ &quot;￥&quot;* &quot;-&quot;??_ ;_ @_ "/>
+    <numFmt numFmtId="43" formatCode="_ * #,##0.00_ ;_ * \-#,##0.00_ ;_ * &quot;-&quot;??_ ;_ @_ "/>
+    <numFmt numFmtId="42" formatCode="_ &quot;￥&quot;* #,##0_ ;_ &quot;￥&quot;* \-#,##0_ ;_ &quot;￥&quot;* &quot;-&quot;_ ;_ @_ "/>
     <numFmt numFmtId="176" formatCode="000000"/>
-    <numFmt numFmtId="44" formatCode="_ &quot;￥&quot;* #,##0.00_ ;_ &quot;￥&quot;* \-#,##0.00_ ;_ &quot;￥&quot;* &quot;-&quot;??_ ;_ @_ "/>
-    <numFmt numFmtId="41" formatCode="_ * #,##0_ ;_ * \-#,##0_ ;_ * &quot;-&quot;_ ;_ @_ "/>
-    <numFmt numFmtId="42" formatCode="_ &quot;￥&quot;* #,##0_ ;_ &quot;￥&quot;* \-#,##0_ ;_ &quot;￥&quot;* &quot;-&quot;_ ;_ @_ "/>
-    <numFmt numFmtId="43" formatCode="_ * #,##0.00_ ;_ * \-#,##0.00_ ;_ * &quot;-&quot;??_ ;_ @_ "/>
   </numFmts>
-  <fonts count="28">
+  <fonts count="27">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -270,13 +356,6 @@
       <scheme val="minor"/>
     </font>
     <font>
-      <sz val="11"/>
-      <color theme="1"/>
-      <name val="宋体"/>
-      <charset val="134"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
       <sz val="12"/>
       <name val="宋体"/>
       <charset val="134"/>
@@ -291,6 +370,13 @@
     </font>
     <font>
       <sz val="11"/>
+      <color theme="0"/>
+      <name val="宋体"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
       <color theme="1"/>
       <name val="宋体"/>
       <charset val="0"/>
@@ -298,14 +384,7 @@
     </font>
     <font>
       <sz val="11"/>
-      <color theme="0"/>
-      <name val="宋体"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF3F3F76"/>
+      <color rgb="FF006100"/>
       <name val="宋体"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -326,6 +405,14 @@
       <scheme val="minor"/>
     </font>
     <font>
+      <b/>
+      <sz val="11"/>
+      <color rgb="FFFFFFFF"/>
+      <name val="宋体"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
       <sz val="11"/>
       <color rgb="FF9C0006"/>
       <name val="宋体"/>
@@ -349,16 +436,9 @@
       <scheme val="minor"/>
     </font>
     <font>
-      <sz val="11"/>
-      <color rgb="FF9C6500"/>
-      <name val="宋体"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
       <b/>
       <sz val="11"/>
-      <color rgb="FF3F3F3F"/>
+      <color rgb="FFFA7D00"/>
       <name val="宋体"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -388,47 +468,46 @@
       <scheme val="minor"/>
     </font>
     <font>
+      <sz val="11"/>
+      <color rgb="FF3F3F76"/>
+      <name val="宋体"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF9C6500"/>
+      <name val="宋体"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FFFA7D00"/>
+      <name val="宋体"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <i/>
+      <sz val="11"/>
+      <color rgb="FF7F7F7F"/>
+      <name val="宋体"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <u/>
+      <sz val="11"/>
+      <color rgb="FF800080"/>
+      <name val="宋体"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
       <b/>
       <sz val="11"/>
-      <color rgb="FFFFFFFF"/>
-      <name val="宋体"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <i/>
-      <sz val="11"/>
-      <color rgb="FF7F7F7F"/>
-      <name val="宋体"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <u/>
-      <sz val="11"/>
-      <color rgb="FF800080"/>
-      <name val="宋体"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FFFA7D00"/>
-      <name val="宋体"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF006100"/>
-      <name val="宋体"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color rgb="FFFA7D00"/>
+      <color rgb="FF3F3F3F"/>
       <name val="宋体"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -455,13 +534,169 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFC6EFCE"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFA5A5A5"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFC7CE"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFFCC"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFF2F2F2"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFCC99"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFEB9C"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
         <fgColor theme="9" tint="0.599993896298105"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="9"/>
+        <fgColor theme="8"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -473,169 +708,13 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor rgb="FFFFCC99"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.599993896298105"/>
+        <fgColor theme="5" tint="0.799981688894314"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
         <fgColor theme="4" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFC7CE"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFFFCC"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFEB9C"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFF2F2F2"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFA5A5A5"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFC6EFCE"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -664,26 +743,26 @@
       <diagonal/>
     </border>
     <border>
-      <left style="thin">
-        <color rgb="FF7F7F7F"/>
-      </left>
-      <right style="thin">
-        <color rgb="FF7F7F7F"/>
-      </right>
-      <top style="thin">
-        <color rgb="FF7F7F7F"/>
-      </top>
-      <bottom style="thin">
-        <color rgb="FF7F7F7F"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
       <left/>
       <right/>
       <top/>
       <bottom style="medium">
         <color theme="4"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="double">
+        <color rgb="FF3F3F3F"/>
+      </left>
+      <right style="double">
+        <color rgb="FF3F3F3F"/>
+      </right>
+      <top style="double">
+        <color rgb="FF3F3F3F"/>
+      </top>
+      <bottom style="double">
+        <color rgb="FF3F3F3F"/>
       </bottom>
       <diagonal/>
     </border>
@@ -715,6 +794,39 @@
     </border>
     <border>
       <left style="thin">
+        <color rgb="FF7F7F7F"/>
+      </left>
+      <right style="thin">
+        <color rgb="FF7F7F7F"/>
+      </right>
+      <top style="thin">
+        <color rgb="FF7F7F7F"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="FF7F7F7F"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="medium">
+        <color theme="4" tint="0.499984740745262"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="double">
+        <color rgb="FFFF8001"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
         <color rgb="FF3F3F3F"/>
       </left>
       <right style="thin">
@@ -728,39 +840,6 @@
       </bottom>
       <diagonal/>
     </border>
-    <border>
-      <left/>
-      <right/>
-      <top/>
-      <bottom style="medium">
-        <color theme="4" tint="0.499984740745262"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="double">
-        <color rgb="FF3F3F3F"/>
-      </left>
-      <right style="double">
-        <color rgb="FF3F3F3F"/>
-      </right>
-      <top style="double">
-        <color rgb="FF3F3F3F"/>
-      </top>
-      <bottom style="double">
-        <color rgb="FF3F3F3F"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
-      <right/>
-      <top/>
-      <bottom style="double">
-        <color rgb="FFFF8001"/>
-      </bottom>
-      <diagonal/>
-    </border>
   </borders>
   <cellStyleXfs count="49">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0">
@@ -769,10 +848,10 @@
     <xf numFmtId="42" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="8" fillId="20" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="6" borderId="2" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="8" fillId="24" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="20" fillId="20" borderId="6" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="44" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
@@ -781,137 +860,137 @@
     <xf numFmtId="41" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="8" fillId="10" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="11" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="8" fillId="7" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="12" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="43" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="9" fillId="25" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="20" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="7" fillId="27" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="9" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="24" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="15" borderId="5" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="11" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="17" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="23" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="15" borderId="5" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="24" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="18" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="19" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="22" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="15" fillId="0" borderId="3" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="0" borderId="3" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="14" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="18" fillId="0" borderId="7" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="17" fillId="19" borderId="6" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="26" fillId="19" borderId="2" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="21" fillId="23" borderId="8" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="15" fillId="0" borderId="2" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="2" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="26" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="17" fillId="0" borderId="7" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="10" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="25" fillId="19" borderId="9" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="19" borderId="6" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="9" borderId="3" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="23" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="22" fillId="0" borderId="8" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="4" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="6" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="21" fillId="22" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="5" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="4" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="21" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="33" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="8" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="25" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="14" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="18" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="13" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="29" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="3" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="17" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="8" fillId="28" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="9" fillId="13" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="24" fillId="0" borderId="9" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="0" borderId="4" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="25" fillId="33" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="16" fillId="18" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="17" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="27" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="22" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="9" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="8" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="26" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="7" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="12" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="21" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="5" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="16" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="4" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="3" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="29" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="7" fillId="16" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="20">
+  <cellXfs count="19">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0">
       <alignment vertical="center"/>
     </xf>
@@ -939,9 +1018,6 @@
     <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="176" fontId="3" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -954,23 +1030,23 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1">
+      <alignment vertical="center"/>
     </xf>
     <xf numFmtId="176" fontId="3" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
     <xf numFmtId="176" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1">
-      <alignment vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="49">
@@ -1321,7 +1397,7 @@
   <dimension ref="A1:I28"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="B1" workbookViewId="0">
-      <selection activeCell="D3" sqref="D3"/>
+      <selection activeCell="E3" sqref="E3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9" defaultRowHeight="14.4"/>
@@ -1369,7 +1445,9 @@
       <c r="A2" s="6" t="s">
         <v>9</v>
       </c>
-      <c r="B2" s="6"/>
+      <c r="B2" s="6">
+        <v>1</v>
+      </c>
       <c r="C2" s="6"/>
       <c r="D2" s="7" t="s">
         <v>10</v>
@@ -1392,61 +1470,75 @@
     </row>
     <row r="3" s="1" customFormat="1" spans="1:9">
       <c r="A3" s="6"/>
-      <c r="B3" s="6"/>
+      <c r="B3" s="6">
+        <v>2</v>
+      </c>
       <c r="C3" s="6"/>
       <c r="D3" s="7" t="s">
         <v>10</v>
       </c>
-      <c r="E3" s="7"/>
-      <c r="F3" s="7"/>
-      <c r="G3" s="7"/>
+      <c r="E3" s="7" t="s">
+        <v>15</v>
+      </c>
+      <c r="F3" s="7">
+        <v>18793172343</v>
+      </c>
+      <c r="G3" s="7" t="s">
+        <v>16</v>
+      </c>
       <c r="H3" s="7"/>
       <c r="I3" s="7"/>
     </row>
     <row r="4" s="1" customFormat="1" ht="15.6" spans="1:9">
       <c r="A4" s="6"/>
-      <c r="B4" s="6"/>
+      <c r="B4" s="6">
+        <v>3</v>
+      </c>
       <c r="C4" s="6"/>
       <c r="D4" s="8" t="s">
-        <v>15</v>
+        <v>17</v>
       </c>
       <c r="E4" s="7" t="s">
-        <v>16</v>
+        <v>18</v>
       </c>
       <c r="F4" s="7">
         <v>15639301768</v>
       </c>
       <c r="G4" s="7" t="s">
-        <v>17</v>
+        <v>19</v>
       </c>
       <c r="H4" s="7"/>
       <c r="I4" s="7"/>
     </row>
     <row r="5" s="1" customFormat="1" ht="15.6" spans="1:9">
       <c r="A5" s="6"/>
-      <c r="B5" s="6"/>
+      <c r="B5" s="6">
+        <v>4</v>
+      </c>
       <c r="C5" s="6"/>
       <c r="D5" s="8" t="s">
-        <v>15</v>
+        <v>17</v>
       </c>
       <c r="E5" s="7" t="s">
-        <v>18</v>
+        <v>20</v>
       </c>
       <c r="F5" s="7">
         <v>15756507454</v>
       </c>
       <c r="G5" s="7" t="s">
-        <v>19</v>
+        <v>21</v>
       </c>
       <c r="H5" s="7"/>
       <c r="I5" s="7"/>
     </row>
     <row r="6" s="1" customFormat="1" ht="15.6" spans="1:9">
       <c r="A6" s="6"/>
-      <c r="B6" s="6"/>
+      <c r="B6" s="6">
+        <v>5</v>
+      </c>
       <c r="C6" s="6"/>
       <c r="D6" s="8" t="s">
-        <v>20</v>
+        <v>22</v>
       </c>
       <c r="E6" s="7"/>
       <c r="F6" s="7"/>
@@ -1456,267 +1548,277 @@
     </row>
     <row r="7" s="1" customFormat="1" ht="15.6" spans="1:9">
       <c r="A7" s="6"/>
-      <c r="B7" s="6"/>
+      <c r="B7" s="6">
+        <v>6</v>
+      </c>
       <c r="C7" s="6"/>
       <c r="D7" s="8" t="s">
-        <v>20</v>
-      </c>
-      <c r="E7" s="9" t="s">
-        <v>21</v>
-      </c>
-      <c r="F7" s="9">
+        <v>23</v>
+      </c>
+      <c r="E7" s="7" t="s">
+        <v>24</v>
+      </c>
+      <c r="F7" s="7">
         <v>17601367477</v>
       </c>
-      <c r="G7" s="9" t="s">
-        <v>22</v>
+      <c r="G7" s="7" t="s">
+        <v>25</v>
       </c>
       <c r="H7" s="7"/>
       <c r="I7" s="7"/>
     </row>
     <row r="8" s="2" customFormat="1" ht="20.4" spans="1:9">
-      <c r="A8" s="10"/>
-      <c r="B8" s="11"/>
-      <c r="C8" s="11"/>
-      <c r="D8" s="12" t="s">
-        <v>23</v>
-      </c>
-      <c r="E8" s="13"/>
-      <c r="F8" s="13"/>
-      <c r="G8" s="13"/>
-      <c r="H8" s="9"/>
-      <c r="I8" s="9"/>
+      <c r="A8" s="9"/>
+      <c r="B8" s="6">
+        <v>7</v>
+      </c>
+      <c r="C8" s="10"/>
+      <c r="D8" s="11" t="s">
+        <v>26</v>
+      </c>
+      <c r="E8" s="12"/>
+      <c r="F8" s="12"/>
+      <c r="G8" s="12"/>
+      <c r="H8" s="7"/>
+      <c r="I8" s="7"/>
     </row>
     <row r="9" s="2" customFormat="1" ht="20.4" spans="1:9">
-      <c r="A9" s="10"/>
-      <c r="B9" s="11"/>
-      <c r="C9" s="11"/>
-      <c r="D9" s="12" t="s">
-        <v>23</v>
-      </c>
-      <c r="E9" s="9" t="s">
-        <v>24</v>
-      </c>
-      <c r="F9" s="9">
+      <c r="A9" s="9"/>
+      <c r="B9" s="6">
+        <v>8</v>
+      </c>
+      <c r="C9" s="10"/>
+      <c r="D9" s="11" t="s">
+        <v>27</v>
+      </c>
+      <c r="E9" s="7" t="s">
+        <v>28</v>
+      </c>
+      <c r="F9" s="7">
         <v>18923874148</v>
       </c>
-      <c r="G9" s="9" t="s">
-        <v>25</v>
-      </c>
-      <c r="H9" s="9"/>
-      <c r="I9" s="9"/>
+      <c r="G9" s="7" t="s">
+        <v>29</v>
+      </c>
+      <c r="H9" s="7"/>
+      <c r="I9" s="7"/>
     </row>
     <row r="10" s="2" customFormat="1" ht="20.4" spans="1:9">
-      <c r="A10" s="10"/>
-      <c r="B10" s="11"/>
-      <c r="C10" s="11"/>
+      <c r="A10" s="9"/>
+      <c r="B10" s="6">
+        <v>9</v>
+      </c>
+      <c r="C10" s="10"/>
       <c r="D10" s="8" t="s">
-        <v>26</v>
-      </c>
-      <c r="E10" s="9" t="s">
-        <v>27</v>
-      </c>
-      <c r="F10" s="9">
+        <v>30</v>
+      </c>
+      <c r="E10" s="7" t="s">
+        <v>31</v>
+      </c>
+      <c r="F10" s="7">
         <v>13930363901</v>
       </c>
-      <c r="G10" s="9" t="s">
-        <v>28</v>
-      </c>
-      <c r="H10" s="9"/>
-      <c r="I10" s="9"/>
+      <c r="G10" s="7" t="s">
+        <v>32</v>
+      </c>
+      <c r="H10" s="7"/>
+      <c r="I10" s="7"/>
     </row>
     <row r="11" s="2" customFormat="1" ht="20.4" spans="1:9">
-      <c r="A11" s="10"/>
-      <c r="B11" s="11"/>
-      <c r="C11" s="11"/>
+      <c r="A11" s="9"/>
+      <c r="B11" s="6">
+        <v>10</v>
+      </c>
+      <c r="C11" s="10"/>
       <c r="D11" s="8" t="s">
-        <v>26</v>
-      </c>
-      <c r="E11" s="9"/>
-      <c r="F11" s="9"/>
-      <c r="G11" s="9"/>
-      <c r="H11" s="9"/>
-      <c r="I11" s="9"/>
+        <v>33</v>
+      </c>
+      <c r="E11" s="7"/>
+      <c r="F11" s="7"/>
+      <c r="G11" s="7"/>
+      <c r="H11" s="7"/>
+      <c r="I11" s="7"/>
     </row>
     <row r="12" s="2" customFormat="1" ht="20.4" spans="1:9">
-      <c r="A12" s="10"/>
-      <c r="B12" s="11"/>
-      <c r="C12" s="11"/>
-      <c r="D12" s="9" t="s">
-        <v>29</v>
-      </c>
-      <c r="E12" s="14" t="s">
-        <v>30</v>
-      </c>
-      <c r="F12" s="14">
+      <c r="A12" s="9"/>
+      <c r="B12" s="6">
+        <v>11</v>
+      </c>
+      <c r="C12" s="10"/>
+      <c r="D12" s="7" t="s">
+        <v>34</v>
+      </c>
+      <c r="E12" s="13" t="s">
+        <v>35</v>
+      </c>
+      <c r="F12" s="13">
         <v>13631120463</v>
       </c>
-      <c r="G12" s="14" t="s">
-        <v>31</v>
-      </c>
-      <c r="H12" s="9"/>
-      <c r="I12" s="9"/>
+      <c r="G12" s="13" t="s">
+        <v>36</v>
+      </c>
+      <c r="H12" s="7"/>
+      <c r="I12" s="7"/>
     </row>
     <row r="13" s="2" customFormat="1" ht="20.4" spans="1:9">
-      <c r="A13" s="10"/>
-      <c r="B13" s="11"/>
-      <c r="C13" s="11"/>
+      <c r="A13" s="9"/>
+      <c r="B13" s="6">
+        <v>12</v>
+      </c>
+      <c r="C13" s="10"/>
       <c r="D13" s="8" t="s">
-        <v>29</v>
-      </c>
-      <c r="E13" s="14" t="s">
-        <v>32</v>
-      </c>
-      <c r="F13" s="14">
+        <v>34</v>
+      </c>
+      <c r="E13" s="13" t="s">
+        <v>37</v>
+      </c>
+      <c r="F13" s="13">
         <v>17850112022</v>
       </c>
-      <c r="G13" s="14" t="s">
-        <v>33</v>
-      </c>
-      <c r="H13" s="9"/>
-      <c r="I13" s="9"/>
+      <c r="G13" s="13" t="s">
+        <v>38</v>
+      </c>
+      <c r="H13" s="7"/>
+      <c r="I13" s="7"/>
     </row>
     <row r="14" s="2" customFormat="1" ht="20.4" spans="1:9">
-      <c r="A14" s="10"/>
-      <c r="B14" s="11"/>
-      <c r="C14" s="11"/>
-      <c r="D14" s="12" t="s">
-        <v>34</v>
-      </c>
-      <c r="E14" s="9"/>
-      <c r="F14" s="9"/>
-      <c r="G14" s="9"/>
-      <c r="H14" s="9"/>
-      <c r="I14" s="9"/>
+      <c r="A14" s="9"/>
+      <c r="B14" s="14"/>
+      <c r="C14" s="14"/>
+      <c r="D14" s="14"/>
+      <c r="E14" s="14"/>
+      <c r="F14" s="14"/>
+      <c r="G14" s="14"/>
+      <c r="H14" s="7"/>
+      <c r="I14" s="7"/>
     </row>
     <row r="15" s="2" customFormat="1" ht="20.4" spans="1:9">
-      <c r="A15" s="10"/>
-      <c r="B15" s="11"/>
-      <c r="C15" s="11"/>
-      <c r="D15" s="12" t="s">
-        <v>34</v>
-      </c>
-      <c r="E15" s="9"/>
-      <c r="F15" s="9"/>
-      <c r="G15" s="9"/>
-      <c r="H15" s="9"/>
-      <c r="I15" s="9"/>
+      <c r="A15" s="9"/>
+      <c r="B15" s="15"/>
+      <c r="C15" s="15"/>
+      <c r="D15" s="15"/>
+      <c r="E15" s="16"/>
+      <c r="F15" s="14"/>
+      <c r="G15" s="14"/>
+      <c r="H15" s="7"/>
+      <c r="I15" s="7"/>
     </row>
     <row r="16" s="3" customFormat="1" ht="8.25" customHeight="1" spans="1:7">
-      <c r="A16" s="15"/>
-      <c r="B16" s="16"/>
-      <c r="C16" s="16"/>
-      <c r="D16" s="16"/>
+      <c r="A16" s="17"/>
+      <c r="B16" s="15"/>
+      <c r="C16" s="15"/>
+      <c r="D16" s="15"/>
       <c r="E16" s="16"/>
-      <c r="F16" s="16"/>
-      <c r="G16" s="16"/>
+      <c r="F16" s="14"/>
+      <c r="G16" s="14"/>
     </row>
     <row r="17" s="3" customFormat="1" ht="20.25" customHeight="1" spans="1:7">
-      <c r="A17" s="17"/>
-      <c r="B17" s="18"/>
-      <c r="C17" s="18"/>
-      <c r="D17" s="18"/>
-      <c r="E17" s="19"/>
-      <c r="F17" s="16"/>
-      <c r="G17" s="16"/>
+      <c r="A17" s="18"/>
+      <c r="B17" s="15"/>
+      <c r="C17" s="15"/>
+      <c r="D17" s="15"/>
+      <c r="E17" s="16"/>
+      <c r="F17" s="14"/>
+      <c r="G17" s="14"/>
     </row>
     <row r="18" s="3" customFormat="1" ht="20.25" customHeight="1" spans="1:7">
-      <c r="A18" s="17"/>
-      <c r="B18" s="18"/>
-      <c r="C18" s="18"/>
-      <c r="D18" s="18"/>
-      <c r="E18" s="19"/>
-      <c r="F18" s="16"/>
-      <c r="G18" s="16"/>
+      <c r="A18" s="18"/>
+      <c r="B18" s="15"/>
+      <c r="C18" s="15"/>
+      <c r="D18" s="15"/>
+      <c r="E18" s="16"/>
+      <c r="F18" s="14"/>
+      <c r="G18" s="14"/>
     </row>
     <row r="19" s="3" customFormat="1" ht="20.25" customHeight="1" spans="1:7">
-      <c r="A19" s="17"/>
-      <c r="B19" s="18"/>
-      <c r="C19" s="18"/>
-      <c r="D19" s="18"/>
-      <c r="E19" s="19"/>
-      <c r="F19" s="16"/>
-      <c r="G19" s="16"/>
+      <c r="A19" s="18"/>
+      <c r="B19" s="15"/>
+      <c r="C19" s="15"/>
+      <c r="D19" s="15"/>
+      <c r="E19" s="16"/>
+      <c r="F19" s="14"/>
+      <c r="G19" s="14"/>
     </row>
     <row r="20" s="3" customFormat="1" ht="20.25" customHeight="1" spans="1:7">
-      <c r="A20" s="17"/>
-      <c r="B20" s="18"/>
-      <c r="C20" s="18"/>
-      <c r="D20" s="18"/>
-      <c r="E20" s="19"/>
-      <c r="F20" s="16"/>
-      <c r="G20" s="16"/>
+      <c r="A20" s="18"/>
+      <c r="B20" s="15"/>
+      <c r="C20" s="15"/>
+      <c r="D20" s="15"/>
+      <c r="E20" s="16"/>
+      <c r="F20" s="14"/>
+      <c r="G20" s="14"/>
     </row>
     <row r="21" s="3" customFormat="1" ht="20.25" customHeight="1" spans="1:7">
-      <c r="A21" s="17"/>
-      <c r="B21" s="18"/>
-      <c r="C21" s="18"/>
-      <c r="D21" s="18"/>
-      <c r="E21" s="19"/>
-      <c r="F21" s="16"/>
-      <c r="G21" s="16"/>
+      <c r="A21" s="18"/>
+      <c r="B21" s="15"/>
+      <c r="C21" s="15"/>
+      <c r="D21" s="15"/>
+      <c r="E21" s="16"/>
+      <c r="F21" s="14"/>
+      <c r="G21" s="14"/>
     </row>
     <row r="22" s="3" customFormat="1" ht="20.25" customHeight="1" spans="1:7">
-      <c r="A22" s="17"/>
-      <c r="B22" s="18"/>
-      <c r="C22" s="18"/>
-      <c r="D22" s="18"/>
-      <c r="E22" s="19"/>
-      <c r="F22" s="16"/>
-      <c r="G22" s="16"/>
+      <c r="A22" s="18"/>
+      <c r="B22" s="15"/>
+      <c r="C22" s="15"/>
+      <c r="D22" s="15"/>
+      <c r="E22" s="16"/>
+      <c r="F22" s="14"/>
+      <c r="G22" s="14"/>
     </row>
     <row r="23" s="3" customFormat="1" ht="20.25" customHeight="1" spans="1:7">
-      <c r="A23" s="17"/>
-      <c r="B23" s="18"/>
-      <c r="C23" s="18"/>
-      <c r="D23" s="18"/>
-      <c r="E23" s="19"/>
-      <c r="F23" s="16"/>
-      <c r="G23" s="16"/>
+      <c r="A23" s="18"/>
+      <c r="B23" s="15"/>
+      <c r="C23" s="15"/>
+      <c r="D23" s="15"/>
+      <c r="E23" s="16"/>
+      <c r="F23" s="14"/>
+      <c r="G23" s="14"/>
     </row>
     <row r="24" s="3" customFormat="1" ht="20.25" customHeight="1" spans="1:7">
-      <c r="A24" s="17"/>
-      <c r="B24" s="18"/>
-      <c r="C24" s="18"/>
-      <c r="D24" s="18"/>
-      <c r="E24" s="19"/>
-      <c r="F24" s="16"/>
-      <c r="G24" s="16"/>
+      <c r="A24" s="18"/>
+      <c r="B24" s="15"/>
+      <c r="C24" s="15"/>
+      <c r="D24" s="15"/>
+      <c r="E24" s="16"/>
+      <c r="F24" s="14"/>
+      <c r="G24" s="14"/>
     </row>
     <row r="25" s="3" customFormat="1" ht="20.25" customHeight="1" spans="1:7">
-      <c r="A25" s="17"/>
-      <c r="B25" s="18"/>
-      <c r="C25" s="18"/>
-      <c r="D25" s="18"/>
-      <c r="E25" s="19"/>
-      <c r="F25" s="16"/>
-      <c r="G25" s="16"/>
+      <c r="A25" s="18"/>
+      <c r="B25" s="15"/>
+      <c r="C25" s="15"/>
+      <c r="D25" s="15"/>
+      <c r="E25" s="16"/>
+      <c r="F25" s="14"/>
+      <c r="G25" s="14"/>
     </row>
     <row r="26" s="3" customFormat="1" ht="20.25" customHeight="1" spans="1:7">
-      <c r="A26" s="17"/>
-      <c r="B26" s="18"/>
-      <c r="C26" s="18"/>
-      <c r="D26" s="18"/>
-      <c r="E26" s="19"/>
-      <c r="F26" s="16"/>
-      <c r="G26" s="16"/>
+      <c r="A26" s="18"/>
+      <c r="B26" s="15"/>
+      <c r="C26" s="15"/>
+      <c r="D26" s="15"/>
+      <c r="E26" s="16"/>
+      <c r="F26" s="14"/>
+      <c r="G26" s="14"/>
     </row>
     <row r="27" s="3" customFormat="1" ht="20.25" customHeight="1" spans="1:7">
-      <c r="A27" s="17"/>
-      <c r="B27" s="18"/>
-      <c r="C27" s="18"/>
-      <c r="D27" s="18"/>
-      <c r="E27" s="19"/>
-      <c r="F27" s="16"/>
-      <c r="G27" s="16"/>
+      <c r="A27" s="18"/>
+      <c r="B27"/>
+      <c r="C27"/>
+      <c r="D27"/>
+      <c r="E27"/>
+      <c r="F27"/>
+      <c r="G27"/>
     </row>
     <row r="28" s="3" customFormat="1" ht="20.25" customHeight="1" spans="1:7">
-      <c r="A28" s="17"/>
-      <c r="B28" s="18"/>
-      <c r="C28" s="18"/>
-      <c r="D28" s="18"/>
-      <c r="E28" s="19"/>
-      <c r="F28" s="16"/>
-      <c r="G28" s="16"/>
+      <c r="A28" s="18"/>
+      <c r="B28"/>
+      <c r="C28"/>
+      <c r="D28"/>
+      <c r="E28"/>
+      <c r="F28"/>
+      <c r="G28"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
rebuilding site Thu Feb 24 18:12:46     2022
</commit_message>
<xml_diff>
--- a/样书_作者(1).xlsx
+++ b/样书_作者(1).xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\study_manger\gitbookHarmonyOS\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1DD83EB1-B32C-41A2-A7D6-32A7B19BF113}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E77CF983-60B9-470A-A14B-7B1595F96646}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -77,6 +77,7 @@
         <sz val="11"/>
         <color rgb="FF333333"/>
         <rFont val="Microsoft YaHei UI"/>
+        <family val="2"/>
         <charset val="134"/>
       </rPr>
       <t>Vue+Spring Boot</t>
@@ -86,6 +87,7 @@
         <sz val="11"/>
         <color rgb="FF333333"/>
         <rFont val="宋体"/>
+        <family val="3"/>
         <charset val="134"/>
       </rPr>
       <t>前后端分离开发实战</t>
@@ -121,6 +123,7 @@
         <sz val="11"/>
         <color rgb="FF333333"/>
         <rFont val="Microsoft YaHei UI"/>
+        <family val="2"/>
         <charset val="134"/>
       </rPr>
       <t>Flutter</t>
@@ -130,6 +133,7 @@
         <sz val="11"/>
         <color rgb="FF333333"/>
         <rFont val="宋体"/>
+        <family val="3"/>
         <charset val="134"/>
       </rPr>
       <t>实战指南</t>
@@ -150,6 +154,7 @@
         <sz val="11"/>
         <color rgb="FF333333"/>
         <rFont val="宋体"/>
+        <family val="3"/>
         <charset val="134"/>
       </rPr>
       <t>实战指南</t>
@@ -179,6 +184,7 @@
         <sz val="11"/>
         <color rgb="FF333333"/>
         <rFont val="Microsoft YaHei UI"/>
+        <family val="2"/>
         <charset val="134"/>
       </rPr>
       <t>HCIA</t>
@@ -188,6 +194,7 @@
         <sz val="11"/>
         <color rgb="FF333333"/>
         <rFont val="宋体"/>
+        <family val="3"/>
         <charset val="134"/>
       </rPr>
       <t>路由与交换技术实战</t>
@@ -203,6 +210,7 @@
         <sz val="11"/>
         <color rgb="FF333333"/>
         <rFont val="宋体"/>
+        <family val="3"/>
         <charset val="134"/>
       </rPr>
       <t>开发入门精要——基于</t>
@@ -212,6 +220,7 @@
         <sz val="11"/>
         <color rgb="FF333333"/>
         <rFont val="Microsoft YaHei UI"/>
+        <family val="2"/>
         <charset val="134"/>
       </rPr>
       <t>Unity</t>
@@ -221,6 +230,7 @@
         <sz val="11"/>
         <color rgb="FF333333"/>
         <rFont val="宋体"/>
+        <family val="3"/>
         <charset val="134"/>
       </rPr>
       <t>和</t>
@@ -230,6 +240,7 @@
         <sz val="11"/>
         <color rgb="FF333333"/>
         <rFont val="Microsoft YaHei UI"/>
+        <family val="2"/>
         <charset val="134"/>
       </rPr>
       <t>MRTK</t>
@@ -257,9 +268,9 @@
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <numFmts count="1">
-    <numFmt numFmtId="178" formatCode="000000"/>
+    <numFmt numFmtId="176" formatCode="000000"/>
   </numFmts>
-  <fonts count="11" x14ac:knownFonts="1">
+  <fonts count="10" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -271,6 +282,7 @@
       <sz val="16"/>
       <color theme="1"/>
       <name val="宋体"/>
+      <family val="3"/>
       <charset val="134"/>
       <scheme val="minor"/>
     </font>
@@ -278,18 +290,21 @@
       <sz val="11"/>
       <color rgb="FF333333"/>
       <name val="Microsoft YaHei UI"/>
+      <family val="2"/>
       <charset val="134"/>
     </font>
     <font>
       <sz val="16"/>
       <color rgb="FFFF0000"/>
       <name val="宋体"/>
+      <family val="3"/>
       <charset val="134"/>
       <scheme val="minor"/>
     </font>
     <font>
       <sz val="12"/>
       <name val="宋体"/>
+      <family val="3"/>
       <charset val="134"/>
       <scheme val="minor"/>
     </font>
@@ -297,6 +312,7 @@
       <sz val="12"/>
       <color rgb="FFFF0000"/>
       <name val="宋体"/>
+      <family val="3"/>
       <charset val="134"/>
       <scheme val="minor"/>
     </font>
@@ -304,6 +320,7 @@
       <sz val="11"/>
       <color rgb="FF333333"/>
       <name val="宋体"/>
+      <family val="3"/>
       <charset val="134"/>
     </font>
     <font>
@@ -320,13 +337,6 @@
       <family val="3"/>
       <charset val="134"/>
       <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF333333"/>
-      <name val="Microsoft YaHei UI"/>
-      <family val="2"/>
-      <charset val="134"/>
     </font>
     <font>
       <sz val="11"/>
@@ -380,7 +390,7 @@
       <alignment vertical="center"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="22">
+  <cellXfs count="21">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0">
       <alignment vertical="center"/>
     </xf>
@@ -393,7 +403,7 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="178" fontId="0" fillId="2" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="176" fontId="0" fillId="2" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -408,7 +418,7 @@
     <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="178" fontId="3" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="176" fontId="3" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
@@ -429,22 +439,19 @@
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="178" fontId="3" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="176" fontId="3" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
-    <xf numFmtId="178" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="176" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="8" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="9" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
@@ -752,7 +759,7 @@
   <dimension ref="A1:I28"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C14" sqref="C14"/>
+      <selection activeCell="D6" sqref="D6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9" defaultRowHeight="13.5" x14ac:dyDescent="0.15"/>
@@ -902,7 +909,7 @@
         <v>5</v>
       </c>
       <c r="C6" s="6"/>
-      <c r="D6" s="19" t="s">
+      <c r="D6" s="8" t="s">
         <v>35</v>
       </c>
       <c r="E6" s="7" t="s">
@@ -930,7 +937,7 @@
       <c r="D7" s="18" t="s">
         <v>34</v>
       </c>
-      <c r="E7" s="20" t="s">
+      <c r="E7" s="19" t="s">
         <v>36</v>
       </c>
       <c r="F7" s="11">
@@ -1005,13 +1012,13 @@
       <c r="D10" s="8" t="s">
         <v>28</v>
       </c>
-      <c r="E10" s="21" t="s">
+      <c r="E10" s="20" t="s">
         <v>38</v>
       </c>
       <c r="F10" s="7">
         <v>17752170152</v>
       </c>
-      <c r="G10" s="21" t="s">
+      <c r="G10" s="20" t="s">
         <v>39</v>
       </c>
       <c r="H10" s="7" t="s">

</xml_diff>